<commit_message>
Fix minor API bug
</commit_message>
<xml_diff>
--- a/results/predictions/Rick Astley - Never Gonna Give You Up (Official Music Video).xlsx
+++ b/results/predictions/Rick Astley - Never Gonna Give You Up (Official Music Video).xlsx
@@ -488,12 +488,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>caring</t>
+          <t>optimism</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>moderate</t>
+          <t>mild</t>
         </is>
       </c>
     </row>
@@ -515,17 +515,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>fear</t>
+          <t>happiness</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>nervousness</t>
+          <t>excitement</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>moderate</t>
+          <t>mild</t>
         </is>
       </c>
     </row>
@@ -547,12 +547,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>optimism</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -579,12 +579,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>curiosity</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>moderate</t>
+          <t>mild</t>
         </is>
       </c>
     </row>

</xml_diff>